<commit_message>
UI modifications, Pagination issue resolved, Interview form required field validation added and bug fixes.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charmdm\Desktop\Oral History\09_25_2018 Patrick Feedback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OralCMS\trunk\src\WpfApp\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="333">
   <si>
     <t>Title</t>
   </si>
@@ -129,6 +129,99 @@
     <t>SOK_256</t>
   </si>
   <si>
+    <t>Transcriber Assigned</t>
+  </si>
+  <si>
+    <t>Transcription Notes</t>
+  </si>
+  <si>
+    <t>Equipment #</t>
+  </si>
+  <si>
+    <t>Metadata Draft</t>
+  </si>
+  <si>
+    <t>Location of Interview</t>
+  </si>
+  <si>
+    <t>Interviewer Description</t>
+  </si>
+  <si>
+    <t>Interviewer Keywords</t>
+  </si>
+  <si>
+    <t>Interviewer Subjects</t>
+  </si>
+  <si>
+    <t>Release Form</t>
+  </si>
+  <si>
+    <t>Restrictions</t>
+  </si>
+  <si>
+    <t>Restriction Notes</t>
+  </si>
+  <si>
+    <t>Recording Format</t>
+  </si>
+  <si>
+    <t>Equipment Used</t>
+  </si>
+  <si>
+    <t>Interviewer Notes</t>
+  </si>
+  <si>
+    <t>Sent Out</t>
+  </si>
+  <si>
+    <t>Transcription Status</t>
+  </si>
+  <si>
+    <t>Access Media Status</t>
+  </si>
+  <si>
+    <t>Born digital</t>
+  </si>
+  <si>
+    <t>On CONTENTdm</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>TF AC, E1, draft mailed 8/17, complete 12/17</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>Miller discusses her writing career and her time hosting/producing the TV show Writing Out Loud.</t>
+  </si>
+  <si>
+    <t>novels, memoirs, television, OETA, Writing Out Loud</t>
+  </si>
+  <si>
+    <t>Gender differences, work environment</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>audio and video</t>
+  </si>
+  <si>
+    <t>Canon X20; Marantz 661</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
     <t>Oral history interview with Frank Kekahbah</t>
   </si>
   <si>
@@ -156,6 +249,24 @@
     <t>SOK_264</t>
   </si>
   <si>
+    <t>TF AC, E1, draft mailed 7/17, complete 9/17</t>
+  </si>
+  <si>
+    <t>Stillwater</t>
+  </si>
+  <si>
+    <t>Ventress spoke about growing up in Stillwater, developing an interest in science and match, deciding to attend OSU, and earning degrees in Chemical Engineering. She also talked about being a woman in a STEM field, experiences along the way, and her thoughts on gender in the workplace. She also discussed competitng in the Highland Athletic Games around the world and her Scottsh heritage.</t>
+  </si>
+  <si>
+    <t>STEM fields, women, work, chemical engineering</t>
+  </si>
+  <si>
+    <t>Natural resources conservation, guernsey cows, erosion</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Oral history interview with Mitchell Cypress</t>
   </si>
   <si>
@@ -177,6 +288,15 @@
     <t>SOK_259</t>
   </si>
   <si>
+    <t xml:space="preserve">Haumpy talks about her experiences in high school at Chilocco and her work for Creek Nation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muscogee Creek, Absentee Shawnee, (town of) Shawnee, arrival at Chilocco, Chilocco cheer team, school dances,  Haskell Junior College, Baker University, University of Oklahoma, Master's degree, self-governance and social services at Creel Matopm  </t>
+  </si>
+  <si>
+    <t>Natural resources conservation, erosion, liberty beans</t>
+  </si>
+  <si>
     <t>Oral history interview with Charley Johnson</t>
   </si>
   <si>
@@ -201,6 +321,21 @@
     <t>SOK_288</t>
   </si>
   <si>
+    <t>Edmond</t>
+  </si>
+  <si>
+    <t>Squires talks about growing up in a military family and how living abroad helped her appreciate Oklahoma. She also discusses her career as a novelist and professor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">novels, rock music, Medicine Park, military </t>
+  </si>
+  <si>
+    <t>Conservation Reserve Program, Water quality, Erosion</t>
+  </si>
+  <si>
+    <t>didn't want video released</t>
+  </si>
+  <si>
     <t>Oral history interview with Charles LeClair</t>
   </si>
   <si>
@@ -225,6 +360,15 @@
     <t>SOK_268</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; MW E2; draft mailed 10/1/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Eaton, a 2018 Tulsa Artist Fellow, talks about her work as an international journalist. We also discuss her nonfiction book which covered small town life in every county of Oklahoma. We end the conversation with her TAF project: interviewing women who are incarcerated in Oklahoma.</t>
+  </si>
+  <si>
+    <t>Natural resources, conservation, youth</t>
+  </si>
+  <si>
     <t>Oral history interview with Bunnie McCosar</t>
   </si>
   <si>
@@ -249,6 +393,15 @@
     <t>SOK_265</t>
   </si>
   <si>
+    <t>Stockel recalled her days as a fire safety and technology student at OSU back in the 1980s, being the second female to go through the program and live in the fire station, and how she became interested in fire safety. She discusses her career, earning a master's degree, and returning to OSU to teach in the program - roughly 30 years later. She also talks about the lack of women in the STEM fields.</t>
+  </si>
+  <si>
+    <t>STEM fields, women, work, safety engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conservation, erosion, equipment </t>
+  </si>
+  <si>
     <t>Oral history interview with John Peacock</t>
   </si>
   <si>
@@ -273,6 +426,21 @@
     <t>SOK_289</t>
   </si>
   <si>
+    <t>Christina (Pract)</t>
+  </si>
+  <si>
+    <t>Oklahoma City</t>
+  </si>
+  <si>
+    <t>Mungle shares his dairy farming background and how he began his involvement in Oklahoma's conservation activities. He discusses his 10 years on the Conservation Commission, some of the issues during his time there, and some of the key people. He also talks about his career with the Farmers Bureau and with a royalty company. 2. Mungle focused on his tenure as executive director of the Oklahoma Conservation Commission, spoke about various commissioners he served with, the process of getting appointed, working with various governors, and some of the politics that goes with the field.</t>
+  </si>
+  <si>
+    <t>FFA, dairy business, mineral royalties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents working at Jones academy, learning basket weaving from her mother in eighth grade, selling her baskets throughout high school in Tahlequah and buying a car, attending NSU and working with her husband in an auditing business, attending Red Earth with her mother, going to North Carolina with her, gathering and weaving with her, quitting baskets while she mourned her mother's passing, being nominated a Cherokee National Treasure, teaching herself the best way to split cane </t>
+  </si>
+  <si>
     <t>Oral history interview with Maurice Howe</t>
   </si>
   <si>
@@ -297,6 +465,18 @@
     <t>SOK_261</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; TF E2; draft mailed 5/18; complete 9/18</t>
+  </si>
+  <si>
+    <t>Stunkard shares his background growing up on a farm on the outskirts of Tulsa, attending OSU, and returning to the Tulsa/Wagoner County area to start farming himself. He discusses getting involved with the Wagoner County Conservation District and his efforts to improve watersheds to prevent or reduce flooding. He also talks about a few of his memories in the farming business and his conversation activities at the state level.</t>
+  </si>
+  <si>
+    <t>4-H, cattle, row crops, flood control</t>
+  </si>
+  <si>
+    <t>Phi Beta Kappa, OSU</t>
+  </si>
+  <si>
     <t>Oral history interview with Nathan Benton</t>
   </si>
   <si>
@@ -321,6 +501,18 @@
     <t>SOK_260</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; TF E2; draft mailed 5/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Clark shares how his grandparents were pioneer ranchers in the Panhandle and how his father came to own the Clark Ranch. He discusses improvements he has made on the land to help protect the topsoil. He also talks about his conservation activities in the Cimarron County Conservation District as well as other conservation of natural resources issues he has supported at the state and national level. He disccuses tillage systems, range management, and water quality.</t>
+  </si>
+  <si>
+    <t>Water, cattle, tillage</t>
+  </si>
+  <si>
+    <t>Independent press, Tulsa, longform journalism</t>
+  </si>
+  <si>
     <t>Oral history interview with Richard Mendez</t>
   </si>
   <si>
@@ -342,6 +534,21 @@
     <t>SOK_266</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; MW E2; draft mailed 10/10/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Walters</t>
+  </si>
+  <si>
+    <t>Hudman talked about his childhood, living in a children's home, and how he came to live in Cotton County. He also talked about his efforts in conservation, assisting the county with building a structure to house the district office, and some of the people he worked with through the yers.</t>
+  </si>
+  <si>
+    <t>tillage, lagoons, county office</t>
+  </si>
+  <si>
+    <t>Growing up in Boston area, loving Boston Red Sox from early age, studying English at Brown, studying writing for MFA at the University of Arkansas, moving to Tahlequah, adjusting to life in Oklahoma, giving writing advice, discussing craft of flash fiction</t>
+  </si>
+  <si>
     <t>Oral history interview with Davene Alford</t>
   </si>
   <si>
@@ -366,6 +573,24 @@
     <t>SOK_255</t>
   </si>
   <si>
+    <t>JPLT AC; RS E1; ready for E2</t>
+  </si>
+  <si>
+    <t>Mooreland</t>
+  </si>
+  <si>
+    <t>Maddux spoke about his start in farming, some of his conservation work, and touched upon his time in the Oklahoma legislature.</t>
+  </si>
+  <si>
+    <t>Farming, family, terraces, farm equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing persona poetry, working with other artists on creative collaborations, teaching poetry at Ghost Ranch, working as a reference librarian </t>
+  </si>
+  <si>
+    <t>Marants pmd621</t>
+  </si>
+  <si>
     <t>Oral history interview with Alfred Frejo</t>
   </si>
   <si>
@@ -390,6 +615,21 @@
     <t>SOK_258</t>
   </si>
   <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kansas, OK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cottrell, a Cherokee National Treasure, talks about her mother's influence on her basketmaking and her love for double-walled weaving with natural materials. </t>
+  </si>
+  <si>
+    <t>Jones Academy, Tahlequah, her mother, Betty Scraper Garner, commercial reed, buckbrush, white oak, honeysuckle, cane, Red Earth Indian Arts Festival, Cherokee National Treaures</t>
+  </si>
+  <si>
+    <t>Adjusting to life in Oklahoma, writing about nature, pursuing interest in birding, working as an arts administrator, studying Emily Dickinson, interacting with Elizabeth Bishop, studying with Harold Bloom</t>
+  </si>
+  <si>
     <t>Oral history interview with T. J. Burris</t>
   </si>
   <si>
@@ -411,6 +651,18 @@
     <t>SOK_254</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; MW E2; draft mailed 10/18/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Hargis discussed his role in OSU being granted a chapter of Phi Beta Kappa. He also spoke about campus improvements and a few of his highlights during his 10 years as president.</t>
+  </si>
+  <si>
+    <t>Honor society, research, campus</t>
+  </si>
+  <si>
+    <t>Industrial engineering, STEM, math</t>
+  </si>
+  <si>
     <t>Oral history interview with Amos Harjo Jr.</t>
   </si>
   <si>
@@ -435,6 +687,18 @@
     <t>SOK_257</t>
   </si>
   <si>
+    <t>Rosalie AC, E1; MW E2; draft mailed 11/15/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mason shares his experiences growing up in Tulsa in the 1970s as the son of Cuban/Peruvian parents. He also shares his college experience at Oral Roberts University and details the events that led him to pursue writing as a profession. Lastly, Mason talks in detail about running and editing This Land Press. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This Land Press, Oral Roberts University, Cuban-American, Tulsa, journalism </t>
+  </si>
+  <si>
+    <t xml:space="preserve">attending Carter Seminary, attending Chilocco, getting in trouble for nighthawking, meeting her husband, workign as an elevator girl one summer, buying new clothes, having to leave Chilocco ecause of a matron's report that she was well of, being visited by the social worker who observed her family was indeed poor and being reinstated at Chilocco, taking in two Seneca boys weekends and holidays while her husband worked in the dairy, working as a head research secretary at OSU while her husband went to school, returning to Chilocco the last decade, her thoughts on Eugene Voigt's death, why Chilocco closed, on the tremendous reputation Chilocco graduates had in Indian country </t>
+  </si>
+  <si>
     <t>Oral history interview with Anile Locust</t>
   </si>
   <si>
@@ -456,6 +720,18 @@
     <t>SOK_287</t>
   </si>
   <si>
+    <t>Tahlequah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murphy, a Boston native, moved to Tahlequah, Oklahoma seven years ago. He earned his MFA from the University of Arkansas and specializes in flash fiction. Murphy discusses his work (and we talk about the craft of flash writing) and he also provides valuable insight into how he has adjusted to living in eastern Oklahoma. </t>
+  </si>
+  <si>
+    <t>Boston, Red Sox, baseball, fiction, flash fiction, Tahlequah</t>
+  </si>
+  <si>
+    <t>Flood control</t>
+  </si>
+  <si>
     <t>Oral history interview with Jim Baker</t>
   </si>
   <si>
@@ -480,6 +756,21 @@
     <t>SOK_252</t>
   </si>
   <si>
+    <t>no audio, MW AC, E1, draft mailed 9/17, complete 5/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taylor discussed her body of work -- including a poetry book called OUR LADY VICTORY which was a semi-autobiographical account of her experience living in a home for unwed mothers in Oklahoma in the late 1960s. She also talked about pursuing a women's study major at OU in the early 1970s, which led her to later study library science. She also shares her experiences working as a poetry teacher at the famous Ghost Ranch in New Mexico. </t>
+  </si>
+  <si>
+    <t>Ghost Ranch, poetry, persona poetry</t>
+  </si>
+  <si>
+    <t>St. John's, Antigua, immigrants, Tulsa, racism, nursing, black nurses, Okemah lynching, Laura Nelson, LD Nelson, Jane Crow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio   </t>
+  </si>
+  <si>
     <t>Oral history interview with Charles Burris</t>
   </si>
   <si>
@@ -504,6 +795,18 @@
     <t>SOK_262</t>
   </si>
   <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kidney talked about her early life and how those experiences (especially with her artistic parents) led her to pursue writing. She shared what Oberlin College was like in the late 1960s (it was not the liberal milieu that it's known as today); she also shared what it was like studying English at Yale in the early 1970s with famous literary critic and scholar, Harold Bloom. Kidney discussed the circumstances that led her to Stillwater, Oklahoma in the late 1970s and how/why she has remained here ever since. Kidney talked about her time as the administrator for Let's Talk About it, Oklahoma. Lastly, she provided her best writing advice -- especially for the writing and study of poetry. </t>
+  </si>
+  <si>
+    <t>poetry, Emily Dickinson, Elizabeth Bishop, Let's Talk About It, Oklahoma, arts administration</t>
+  </si>
+  <si>
+    <t>Vietnam war, Vietnam veteran, poetry</t>
+  </si>
+  <si>
     <t>Oral history interview with Dean Hudson</t>
   </si>
   <si>
@@ -528,6 +831,18 @@
     <t>SOK_267</t>
   </si>
   <si>
+    <t>RS AC, E1; ready for E2</t>
+  </si>
+  <si>
+    <t>Dibble shared her journey to becoming an industrial engineer. She talks about her time at OSU, her first job, and coming into her own. She also offers advice and suggestions for young people, women in particular, who are interested in the field.</t>
+  </si>
+  <si>
+    <t>Women in the workforce, education, aspiration</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
     <t>Oral history interview with Robert Buzzard</t>
   </si>
   <si>
@@ -552,6 +867,18 @@
     <t>SOK_296</t>
   </si>
   <si>
+    <t>RS AC, E1; in w/MW</t>
+  </si>
+  <si>
+    <t>Newkirk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King, class of 52, talks about her thirty year history with Chilocco Indian School as a student and employee who worked there during two separate periods, including Chilocc's closing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ada, Chickasaw, Carter Seminary, Chilocco,  Korean war, Oklahoma State University. Newkirk, Navajo program, Eugene Voigt,  Chilocco Hall of Fame speech, </t>
+  </si>
+  <si>
     <t>Oral history interview with Joe Thornton</t>
   </si>
   <si>
@@ -579,6 +906,18 @@
     <t>SOK_286</t>
   </si>
   <si>
+    <t>RS AC, E1; TF E2; draft mailed 5/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Perry, OK</t>
+  </si>
+  <si>
+    <t>Imgarten, born in 1928, discusses growing up on a farm, attending a one-room school for grades up to eighth, and talks some about high school. He talks about being a 50+ year board member for the Red Rock Conservancy District, negotiating for easements, and the value of watershed projects and dams.</t>
+  </si>
+  <si>
+    <t>flooding, landowners, easements, Henry Bellmon, H.E. Bailey</t>
+  </si>
+  <si>
     <t>Oral history interview with George England</t>
   </si>
   <si>
@@ -603,73 +942,16 @@
     <t>SOK_295</t>
   </si>
   <si>
-    <t>Oral history interview with Charles Chupco</t>
-  </si>
-  <si>
-    <t>Chupco, Charles</t>
-  </si>
-  <si>
-    <t>Indians of North America; Chilocco Indian Agricultural School; Chilocco Indian Agricultural School--Alumni and alumnae; Indians of North America--Education; Off-reservation boarding schools; Boarding school students; United States. National Guard Bureau; Indians of North America--Wars--Veterans; United States. Navy; Vietnam War (1961-1975)</t>
-  </si>
-  <si>
-    <t>Charles Chupco (Creek), a 1960 graduate of Chilocco Indian Agricultural School, talks about his time on campus and some of his memories as a student, like working in auto mechanics and participating in multiple sports. He mentions his Creek heritage and how it was nice having Creek classmates. Chupco shares why he joined the Navy after briefly being part of the National Guard at Chilocco. He discusses his twenty-year military career, serving on various ships in different locations. Chupco also talks about his post-military career and some of his duties in technical operations for a school district.</t>
-  </si>
-  <si>
-    <t>Newkirk, Oklahoma; Yokosuka, Japan; San Diego, California; Austin, Texas</t>
-  </si>
-  <si>
-    <t>1948-2017</t>
-  </si>
-  <si>
-    <t>SOK_308</t>
-  </si>
-  <si>
-    <t>Oral history interview with Keith Franklin</t>
-  </si>
-  <si>
-    <t>Franklin, Keith</t>
-  </si>
-  <si>
-    <t>Indians of North America; Chilocco Indian Agricultural School; Chilocco Indian Agricultural School--Alumni and alumnae; Indians of North America--Education; Off-reservation boarding schools; Boarding school students; Indians of North America--Wars--Veterans; United States. Air Force; Vietnam War (1961-1975)</t>
-  </si>
-  <si>
-    <t>Military experience</t>
-  </si>
-  <si>
-    <t>Keith Franklin (Sac and Fox), a 1957 graduate of Chilocco Indian Agricultural School, talks about his journey to Chilocco and some of his early challenges with boarding school life. He describes a few of his memories from his time there as a student and the vocational work he had to do. Franklin enlisted in the U.S. Air Force and goes through his twenty-three-year military career, commenting on experiences he had and the things that he saw, both good and bad. He mentions some of the more dangerous parts of his military duties and how that danger affected him personally and those around him. Franklin shares his opinion about his military duties and the impact of the U.S. in the areas he was serving in, specifically Guam and Thailand. He also talks about how his time at Chilocco affected his time in the military.</t>
-  </si>
-  <si>
-    <t>Newkirk, Oklahoma; Guam; Thailand</t>
-  </si>
-  <si>
-    <t>1946-2017</t>
-  </si>
-  <si>
-    <t>SOK_307</t>
-  </si>
-  <si>
-    <t>Oral history interview with Art Hill, Jr.</t>
-  </si>
-  <si>
-    <t>Hill, Art, Jr.</t>
-  </si>
-  <si>
-    <t>Nykolaiszyn, Juliana</t>
-  </si>
-  <si>
-    <t>Indians of North America; Chilocco Indian Agricultural School; Chilocco Indian Agricultural School--Alumni and alumae; Indians of North America--Education; Off-reservation boarding schools; Boarding school students; United States. National Guard Bureau; United States. Army; Indians of North America--Wars--Veterans</t>
-  </si>
-  <si>
-    <t>Military experience; Race prejudice</t>
-  </si>
-  <si>
-    <t>Art Hill, Jr. (Cheyenne and Oneida) attended Chilocco Indian Agricultural School 1979-1980, his freshman year in high school. He talks about his father's connection to Chilocco and his own decision to enroll in the school. Hill shares some of his memories of Chilocco such as being on the football team, learning self-discipline, and taking classes in automobile mechanics. He explains why he joined the military and recalls some of his specific duties. Hill comments on some of the challenges he faced as an Indian man in the military and how that impacted his experiences. He also notes his continued connection to Chilocco.</t>
-  </si>
-  <si>
-    <t>Newkirk, Oklahoma; Kansas; Hohenfels, Germany</t>
-  </si>
-  <si>
-    <t>1971-2017</t>
+    <t>RS AC, E1; E2 TF;draft mailed 7/11/18; complete 11/18</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>Pasley, born in St. John’s, Antigua, moved to Tulsa, Oklahoma, as a young child and grew up in the Greenwood area. She talks about her path to earning an MFA in Creative Nonfiction writing, and the project she started working on in graduate school that involves the May 25, 1911 lynching of Laura and LD Nelson in Okemah. She also discusses her career as a nurse and the racist interactions with patients she encountered on the job.</t>
+  </si>
+  <si>
+    <t>Canon X20; Marantz 662</t>
   </si>
   <si>
     <t>Oral history interview with Claudine King</t>
@@ -696,6 +978,15 @@
     <t>SOK_347</t>
   </si>
   <si>
+    <t>Bartolina spoke about his youth in Colton, Oklahoma, attending Oklahoma A &amp; M/OSU, and how he got involved with conservation. He discussed his various roles from conducting soil surveys to managing the National Land &amp; Range Judging contest.</t>
+  </si>
+  <si>
+    <t>soils, landowners, urban, student contests</t>
+  </si>
+  <si>
+    <t>conservation, watersheds, soil surveys</t>
+  </si>
+  <si>
     <t>Oral history interview with Virginia McDonald Rush</t>
   </si>
   <si>
@@ -718,6 +1009,15 @@
   </si>
   <si>
     <t>SOK_299</t>
+  </si>
+  <si>
+    <t>Hodges spoke about her youth during the Dust Bowl in Beaver County, Oklahoma, about her early education, the struggles her parents had, and how she pursued a college education. She spoke about being involved with the Ken Burns film on the Dust Bowl, participating in a Readers Theater, and conducting research for books on the history of the panhandle area.</t>
+  </si>
+  <si>
+    <t>childhood, dust bowl, wpa, education</t>
+  </si>
+  <si>
+    <t>conservation, Ken Burns, teaching, authorship</t>
   </si>
 </sst>
 </file>
@@ -1201,9 +1501,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1525,72 +1829,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="32.7109375" customWidth="1"/>
+    <col min="26" max="26" width="61.7109375" customWidth="1"/>
+    <col min="27" max="27" width="34.7109375" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31" customWidth="1"/>
+    <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1645,28 +2019,82 @@
       <c r="S2" t="s">
         <v>35</v>
       </c>
+      <c r="T2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
-        <v>42517</v>
+        <v>42518</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
         <v>25</v>
@@ -1687,10 +2115,10 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
         <v>33</v>
@@ -1699,30 +2127,84 @@
         <v>34</v>
       </c>
       <c r="S3" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="T3" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1">
-        <v>42518</v>
+        <v>42517</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -1743,10 +2225,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="Q4" t="s">
         <v>33</v>
@@ -1755,30 +2237,84 @@
         <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>51</v>
+        <v>75</v>
+      </c>
+      <c r="T4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>42678</v>
+        <v>42518</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -1799,10 +2335,10 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
         <v>33</v>
@@ -1811,30 +2347,84 @@
         <v>34</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>88</v>
+      </c>
+      <c r="T5" t="s">
+        <v>55</v>
+      </c>
+      <c r="U5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
-        <v>42518</v>
+        <v>42678</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -1855,10 +2445,10 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="Q6" t="s">
         <v>33</v>
@@ -1867,30 +2457,87 @@
         <v>34</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>99</v>
+      </c>
+      <c r="T6" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6">
+        <v>4</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
       <c r="D7" s="1">
-        <v>42517</v>
+        <v>42518</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
@@ -1911,10 +2558,10 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="P7" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="Q7" t="s">
         <v>33</v>
@@ -1923,30 +2570,81 @@
         <v>34</v>
       </c>
       <c r="S7" t="s">
-        <v>75</v>
+        <v>112</v>
+      </c>
+      <c r="T7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" t="s">
+        <v>113</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D8" s="1">
-        <v>42719</v>
+        <v>42517</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
@@ -1967,10 +2665,10 @@
         <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="P8" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="Q8" t="s">
         <v>33</v>
@@ -1979,30 +2677,84 @@
         <v>34</v>
       </c>
       <c r="S8" t="s">
-        <v>83</v>
+        <v>123</v>
+      </c>
+      <c r="T8" t="s">
+        <v>55</v>
+      </c>
+      <c r="U8" t="s">
+        <v>56</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1">
-        <v>42517</v>
+        <v>42719</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="I9" t="s">
         <v>25</v>
@@ -2023,10 +2775,10 @@
         <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="P9" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="Q9" t="s">
         <v>33</v>
@@ -2035,30 +2787,84 @@
         <v>34</v>
       </c>
       <c r="S9" t="s">
-        <v>91</v>
+        <v>134</v>
+      </c>
+      <c r="T9" t="s">
+        <v>135</v>
+      </c>
+      <c r="U9" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1">
-        <v>42518</v>
+        <v>42517</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
@@ -2079,10 +2885,10 @@
         <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="P10" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="Q10" t="s">
         <v>33</v>
@@ -2091,30 +2897,84 @@
         <v>34</v>
       </c>
       <c r="S10" t="s">
-        <v>99</v>
+        <v>147</v>
+      </c>
+      <c r="T10" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" t="s">
+        <v>148</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
-        <v>42517</v>
+        <v>42518</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>
@@ -2135,10 +2995,10 @@
         <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="P11" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="Q11" t="s">
         <v>33</v>
@@ -2147,30 +3007,81 @@
         <v>34</v>
       </c>
       <c r="S11" t="s">
-        <v>106</v>
+        <v>159</v>
+      </c>
+      <c r="T11" t="s">
+        <v>55</v>
+      </c>
+      <c r="U11" t="s">
+        <v>160</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X11" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1">
+        <v>42517</v>
+      </c>
+      <c r="F12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1">
-        <v>42518</v>
-      </c>
-      <c r="F12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" t="s">
-        <v>110</v>
-      </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="I12" t="s">
         <v>25</v>
@@ -2191,10 +3102,10 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="P12" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="Q12" t="s">
         <v>33</v>
@@ -2203,30 +3114,84 @@
         <v>34</v>
       </c>
       <c r="S12" t="s">
-        <v>114</v>
+        <v>170</v>
+      </c>
+      <c r="T12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" t="s">
+        <v>171</v>
+      </c>
+      <c r="V12">
+        <v>4</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1">
-        <v>42517</v>
+        <v>42518</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="I13" t="s">
         <v>25</v>
@@ -2247,10 +3212,10 @@
         <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="P13" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="Q13" t="s">
         <v>33</v>
@@ -2259,30 +3224,84 @@
         <v>34</v>
       </c>
       <c r="S13" t="s">
-        <v>122</v>
+        <v>183</v>
+      </c>
+      <c r="T13" t="s">
+        <v>55</v>
+      </c>
+      <c r="U13" t="s">
+        <v>184</v>
+      </c>
+      <c r="V13">
+        <v>3</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X13" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>189</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="1">
-        <v>42518</v>
+        <v>42517</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="G14" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="I14" t="s">
         <v>25</v>
@@ -2303,10 +3322,10 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>128</v>
+        <v>195</v>
       </c>
       <c r="P14" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
       <c r="Q14" t="s">
         <v>33</v>
@@ -2315,15 +3334,69 @@
         <v>34</v>
       </c>
       <c r="S14" t="s">
-        <v>129</v>
+        <v>197</v>
+      </c>
+      <c r="T14" t="s">
+        <v>198</v>
+      </c>
+      <c r="U14" t="s">
+        <v>148</v>
+      </c>
+      <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X14" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>189</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -2332,13 +3405,13 @@
         <v>42518</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="H15" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
@@ -2359,10 +3432,10 @@
         <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>135</v>
+        <v>208</v>
       </c>
       <c r="P15" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="Q15" t="s">
         <v>33</v>
@@ -2371,30 +3444,84 @@
         <v>34</v>
       </c>
       <c r="S15" t="s">
-        <v>137</v>
+        <v>209</v>
+      </c>
+      <c r="T15" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" t="s">
+        <v>210</v>
+      </c>
+      <c r="V15">
+        <v>4</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="1">
-        <v>42636</v>
+        <v>42518</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="G16" t="s">
-        <v>141</v>
+        <v>217</v>
       </c>
       <c r="H16" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="I16" t="s">
         <v>25</v>
@@ -2415,10 +3542,10 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="P16" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
       <c r="Q16" t="s">
         <v>33</v>
@@ -2427,30 +3554,84 @@
         <v>34</v>
       </c>
       <c r="S16" t="s">
-        <v>144</v>
+        <v>221</v>
+      </c>
+      <c r="T16" t="s">
+        <v>55</v>
+      </c>
+      <c r="U16" t="s">
+        <v>222</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>226</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="1">
-        <v>42472</v>
+        <v>42636</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>228</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="H17" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="I17" t="s">
         <v>25</v>
@@ -2471,10 +3652,10 @@
         <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="P17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="Q17" t="s">
         <v>33</v>
@@ -2483,30 +3664,84 @@
         <v>34</v>
       </c>
       <c r="S17" t="s">
-        <v>152</v>
+        <v>232</v>
+      </c>
+      <c r="T17" t="s">
+        <v>198</v>
+      </c>
+      <c r="U17" t="s">
+        <v>56</v>
+      </c>
+      <c r="V17">
+        <v>3</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X17" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="1">
-        <v>42517</v>
+        <v>42472</v>
       </c>
       <c r="F18" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="G18" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
       <c r="H18" t="s">
-        <v>157</v>
+        <v>241</v>
       </c>
       <c r="I18" t="s">
         <v>25</v>
@@ -2527,10 +3762,10 @@
         <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="P18" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="Q18" t="s">
         <v>33</v>
@@ -2539,30 +3774,84 @@
         <v>34</v>
       </c>
       <c r="S18" t="s">
-        <v>160</v>
+        <v>244</v>
+      </c>
+      <c r="T18" t="s">
+        <v>55</v>
+      </c>
+      <c r="U18" t="s">
+        <v>245</v>
+      </c>
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X18" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>246</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>249</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1">
-        <v>42518</v>
+        <v>42517</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>252</v>
       </c>
       <c r="G19" t="s">
-        <v>164</v>
+        <v>253</v>
       </c>
       <c r="H19" t="s">
-        <v>165</v>
+        <v>254</v>
       </c>
       <c r="I19" t="s">
         <v>25</v>
@@ -2583,10 +3872,10 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>166</v>
+        <v>255</v>
       </c>
       <c r="P19" t="s">
-        <v>167</v>
+        <v>256</v>
       </c>
       <c r="Q19" t="s">
         <v>33</v>
@@ -2595,30 +3884,81 @@
         <v>34</v>
       </c>
       <c r="S19" t="s">
-        <v>168</v>
+        <v>257</v>
+      </c>
+      <c r="T19" t="s">
+        <v>55</v>
+      </c>
+      <c r="U19" t="s">
+        <v>184</v>
+      </c>
+      <c r="V19">
+        <v>4</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X19" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>249</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>262</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1">
-        <v>42833</v>
+        <v>42518</v>
       </c>
       <c r="F20" t="s">
-        <v>171</v>
+        <v>264</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="H20" t="s">
-        <v>173</v>
+        <v>266</v>
       </c>
       <c r="I20" t="s">
         <v>25</v>
@@ -2639,10 +3979,10 @@
         <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>174</v>
+        <v>267</v>
       </c>
       <c r="P20" t="s">
-        <v>175</v>
+        <v>268</v>
       </c>
       <c r="Q20" t="s">
         <v>33</v>
@@ -2651,30 +3991,78 @@
         <v>34</v>
       </c>
       <c r="S20" t="s">
-        <v>176</v>
+        <v>269</v>
+      </c>
+      <c r="T20" t="s">
+        <v>55</v>
+      </c>
+      <c r="U20" t="s">
+        <v>270</v>
+      </c>
+      <c r="V20">
+        <v>2</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>274</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1">
-        <v>42636</v>
+        <v>42833</v>
       </c>
       <c r="F21" t="s">
-        <v>180</v>
+        <v>276</v>
       </c>
       <c r="G21" t="s">
-        <v>181</v>
+        <v>277</v>
       </c>
       <c r="H21" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
       <c r="I21" t="s">
         <v>25</v>
@@ -2695,10 +4083,10 @@
         <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="P21" t="s">
-        <v>184</v>
+        <v>280</v>
       </c>
       <c r="Q21" t="s">
         <v>33</v>
@@ -2707,30 +4095,78 @@
         <v>34</v>
       </c>
       <c r="S21" t="s">
-        <v>185</v>
+        <v>281</v>
+      </c>
+      <c r="T21" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" t="s">
+        <v>282</v>
+      </c>
+      <c r="V21">
+        <v>4</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X21" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>285</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>286</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>287</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>288</v>
       </c>
       <c r="D22" s="1">
-        <v>42833</v>
+        <v>42636</v>
       </c>
       <c r="F22" t="s">
-        <v>188</v>
+        <v>289</v>
       </c>
       <c r="G22" t="s">
-        <v>189</v>
+        <v>290</v>
       </c>
       <c r="H22" t="s">
-        <v>190</v>
+        <v>291</v>
       </c>
       <c r="I22" t="s">
         <v>25</v>
@@ -2751,10 +4187,10 @@
         <v>30</v>
       </c>
       <c r="O22" t="s">
-        <v>191</v>
+        <v>292</v>
       </c>
       <c r="P22" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
       <c r="Q22" t="s">
         <v>33</v>
@@ -2763,30 +4199,78 @@
         <v>34</v>
       </c>
       <c r="S22" t="s">
-        <v>193</v>
+        <v>294</v>
+      </c>
+      <c r="T22" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" t="s">
+        <v>295</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X22" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>298</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>194</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s">
-        <v>195</v>
+        <v>300</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>42903</v>
+        <v>42833</v>
       </c>
       <c r="F23" t="s">
-        <v>196</v>
+        <v>301</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>302</v>
       </c>
       <c r="H23" t="s">
-        <v>197</v>
+        <v>303</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -2807,10 +4291,10 @@
         <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>198</v>
+        <v>304</v>
       </c>
       <c r="P23" t="s">
-        <v>199</v>
+        <v>305</v>
       </c>
       <c r="Q23" t="s">
         <v>33</v>
@@ -2819,30 +4303,81 @@
         <v>34</v>
       </c>
       <c r="S23" t="s">
-        <v>200</v>
+        <v>306</v>
+      </c>
+      <c r="T23" t="s">
+        <v>198</v>
+      </c>
+      <c r="U23" t="s">
+        <v>307</v>
+      </c>
+      <c r="V23">
+        <v>3</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X23" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>311</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>312</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1">
-        <v>42902</v>
+        <v>43192</v>
       </c>
       <c r="F24" t="s">
-        <v>203</v>
+        <v>313</v>
       </c>
       <c r="G24" t="s">
-        <v>204</v>
+        <v>314</v>
       </c>
       <c r="H24" t="s">
-        <v>205</v>
+        <v>315</v>
       </c>
       <c r="I24" t="s">
         <v>25</v>
@@ -2863,10 +4398,10 @@
         <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>206</v>
+        <v>316</v>
       </c>
       <c r="P24" t="s">
-        <v>207</v>
+        <v>317</v>
       </c>
       <c r="Q24" t="s">
         <v>33</v>
@@ -2875,30 +4410,81 @@
         <v>34</v>
       </c>
       <c r="S24" t="s">
-        <v>208</v>
+        <v>318</v>
+      </c>
+      <c r="T24" t="s">
+        <v>198</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X24" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>310</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>322</v>
       </c>
       <c r="B25" t="s">
-        <v>210</v>
+        <v>323</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1">
-        <v>42902</v>
+        <v>42857</v>
       </c>
       <c r="F25" t="s">
-        <v>212</v>
+        <v>324</v>
       </c>
       <c r="G25" t="s">
-        <v>213</v>
+        <v>325</v>
       </c>
       <c r="H25" t="s">
-        <v>214</v>
+        <v>326</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
@@ -2919,10 +4505,10 @@
         <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>215</v>
+        <v>327</v>
       </c>
       <c r="P25" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="Q25" t="s">
         <v>33</v>
@@ -2931,119 +4517,58 @@
         <v>34</v>
       </c>
       <c r="S25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>217</v>
-      </c>
-      <c r="B26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="1">
-        <v>43192</v>
-      </c>
-      <c r="F26" t="s">
-        <v>219</v>
-      </c>
-      <c r="G26" t="s">
-        <v>220</v>
-      </c>
-      <c r="H26" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" t="s">
-        <v>27</v>
-      </c>
-      <c r="L26" t="s">
-        <v>28</v>
-      </c>
-      <c r="M26" t="s">
-        <v>29</v>
-      </c>
-      <c r="N26" t="s">
-        <v>30</v>
-      </c>
-      <c r="O26" t="s">
-        <v>222</v>
-      </c>
-      <c r="P26" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>33</v>
-      </c>
-      <c r="R26" t="s">
-        <v>34</v>
-      </c>
-      <c r="S26" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>225</v>
-      </c>
-      <c r="B27" t="s">
-        <v>226</v>
-      </c>
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="1">
-        <v>42857</v>
-      </c>
-      <c r="F27" t="s">
-        <v>227</v>
-      </c>
-      <c r="G27" t="s">
-        <v>228</v>
-      </c>
-      <c r="H27" t="s">
-        <v>229</v>
-      </c>
-      <c r="I27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O27" t="s">
-        <v>230</v>
-      </c>
-      <c r="P27" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>33</v>
-      </c>
-      <c r="R27" t="s">
-        <v>34</v>
-      </c>
-      <c r="S27" t="s">
-        <v>232</v>
+        <v>329</v>
+      </c>
+      <c r="T25" t="s">
+        <v>198</v>
+      </c>
+      <c r="V25">
+        <v>4</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X25" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>330</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>310</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
top menu, filter interviewer list , Audio video equipment adding, sorting and searching in lists and bug fixes.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="334">
   <si>
     <t>Title</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Recording Format</t>
   </si>
   <si>
-    <t>Equipment Used</t>
-  </si>
-  <si>
     <t>Interviewer Notes</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>audio and video</t>
   </si>
   <si>
-    <t>Canon X20; Marantz 661</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -951,9 +945,6 @@
     <t>Pasley, born in St. John’s, Antigua, moved to Tulsa, Oklahoma, as a young child and grew up in the Greenwood area. She talks about her path to earning an MFA in Creative Nonfiction writing, and the project she started working on in graduate school that involves the May 25, 1911 lynching of Laura and LD Nelson in Okemah. She also discusses her career as a nurse and the racist interactions with patients she encountered on the job.</t>
   </si>
   <si>
-    <t>Canon X20; Marantz 662</t>
-  </si>
-  <si>
     <t>Oral history interview with Claudine King</t>
   </si>
   <si>
@@ -1018,6 +1009,18 @@
   </si>
   <si>
     <t>conservation, Ken Burns, teaching, authorship</t>
+  </si>
+  <si>
+    <t>Audio Equipment Used</t>
+  </si>
+  <si>
+    <t>Video Equipment Used</t>
+  </si>
+  <si>
+    <t>Canon X20</t>
+  </si>
+  <si>
+    <t>Marantz 661</t>
   </si>
 </sst>
 </file>
@@ -1829,15 +1832,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL25"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:W25"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF29" sqref="AF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="32.7109375" customWidth="1"/>
@@ -1846,9 +1850,11 @@
     <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="31" customWidth="1"/>
     <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1943,28 +1949,31 @@
         <v>47</v>
       </c>
       <c r="AF1" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2020,61 +2029,64 @@
         <v>35</v>
       </c>
       <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
         <v>55</v>
-      </c>
-      <c r="U2" t="s">
-        <v>56</v>
       </c>
       <c r="V2">
         <v>3</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" t="s">
         <v>57</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>58</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>60</v>
       </c>
-      <c r="AA2" t="s">
-        <v>61</v>
-      </c>
       <c r="AB2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH2" t="s">
         <v>64</v>
       </c>
-      <c r="AF2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>62</v>
-      </c>
       <c r="AI2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AK2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL2" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2130,81 +2142,84 @@
         <v>35</v>
       </c>
       <c r="T3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" t="s">
         <v>55</v>
-      </c>
-      <c r="U3" t="s">
-        <v>56</v>
       </c>
       <c r="V3">
         <v>3</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" t="s">
         <v>57</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>58</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>59</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>60</v>
       </c>
-      <c r="AA3" t="s">
-        <v>61</v>
-      </c>
       <c r="AB3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE3" t="s">
         <v>63</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH3" t="s">
         <v>64</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AI3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="AH3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
       </c>
       <c r="D4" s="1">
         <v>42517</v>
       </c>
       <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
         <v>70</v>
-      </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s">
-        <v>72</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -2225,10 +2240,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q4" t="s">
         <v>33</v>
@@ -2237,69 +2252,72 @@
         <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V4">
         <v>3</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" t="s">
         <v>77</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>78</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH4" t="s">
         <v>79</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AI4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="AB4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="B5" t="s">
         <v>81</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -2308,13 +2326,13 @@
         <v>42518</v>
       </c>
       <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
         <v>84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" t="s">
-        <v>86</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -2335,7 +2353,7 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P5" t="s">
         <v>32</v>
@@ -2347,69 +2365,72 @@
         <v>34</v>
       </c>
       <c r="S5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="T5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" t="s">
         <v>55</v>
-      </c>
-      <c r="U5" t="s">
-        <v>56</v>
       </c>
       <c r="V5">
         <v>2</v>
       </c>
       <c r="W5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" t="s">
         <v>57</v>
       </c>
-      <c r="X5" t="s">
-        <v>58</v>
-      </c>
       <c r="Y5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA5" t="s">
         <v>89</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>90</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="B6" t="s">
         <v>91</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -2418,13 +2439,13 @@
         <v>42678</v>
       </c>
       <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" t="s">
         <v>94</v>
-      </c>
-      <c r="G6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" t="s">
-        <v>96</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -2445,10 +2466,10 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q6" t="s">
         <v>33</v>
@@ -2457,87 +2478,90 @@
         <v>34</v>
       </c>
       <c r="S6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" t="s">
         <v>55</v>
-      </c>
-      <c r="U6" t="s">
-        <v>56</v>
       </c>
       <c r="V6">
         <v>4</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z6" t="s">
         <v>100</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>101</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD6" t="s">
         <v>102</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AE6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>103</v>
       </c>
-      <c r="AB6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD6" t="s">
+      <c r="B7" t="s">
         <v>104</v>
       </c>
-      <c r="AE6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
-      </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1">
         <v>42518</v>
       </c>
       <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" t="s">
         <v>107</v>
-      </c>
-      <c r="G7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" t="s">
-        <v>109</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
@@ -2558,10 +2582,10 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q7" t="s">
         <v>33</v>
@@ -2570,81 +2594,84 @@
         <v>34</v>
       </c>
       <c r="S7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="V7">
         <v>4</v>
       </c>
       <c r="W7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X7" t="s">
         <v>57</v>
       </c>
-      <c r="X7" t="s">
-        <v>58</v>
-      </c>
       <c r="Y7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>114</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="B8" t="s">
         <v>115</v>
       </c>
-      <c r="AB7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>42517</v>
       </c>
       <c r="F8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" t="s">
         <v>118</v>
-      </c>
-      <c r="G8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H8" t="s">
-        <v>120</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
@@ -2665,10 +2692,10 @@
         <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q8" t="s">
         <v>33</v>
@@ -2677,69 +2704,72 @@
         <v>34</v>
       </c>
       <c r="S8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="T8" t="s">
+        <v>54</v>
+      </c>
+      <c r="U8" t="s">
         <v>55</v>
-      </c>
-      <c r="U8" t="s">
-        <v>56</v>
       </c>
       <c r="V8">
         <v>3</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y8" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA8" t="s">
         <v>124</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>125</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="B9" t="s">
         <v>126</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" t="s">
-        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -2748,13 +2778,13 @@
         <v>42719</v>
       </c>
       <c r="F9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" t="s">
         <v>129</v>
-      </c>
-      <c r="G9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" t="s">
-        <v>131</v>
       </c>
       <c r="I9" t="s">
         <v>25</v>
@@ -2775,10 +2805,10 @@
         <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q9" t="s">
         <v>33</v>
@@ -2787,69 +2817,72 @@
         <v>34</v>
       </c>
       <c r="S9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="U9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V9">
         <v>4</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X9" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z9" t="s">
         <v>136</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AA9" t="s">
         <v>137</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AB9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>138</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="B10" t="s">
         <v>139</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" t="s">
-        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -2858,13 +2891,13 @@
         <v>42517</v>
       </c>
       <c r="F10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" t="s">
         <v>142</v>
-      </c>
-      <c r="G10" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" t="s">
-        <v>144</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
@@ -2885,10 +2918,10 @@
         <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Q10" t="s">
         <v>33</v>
@@ -2897,69 +2930,72 @@
         <v>34</v>
       </c>
       <c r="S10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="T10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V10">
         <v>4</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y10" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA10" t="s">
         <v>149</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AB10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>150</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="B11" t="s">
         <v>151</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>153</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -2968,13 +3004,13 @@
         <v>42518</v>
       </c>
       <c r="F11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" t="s">
         <v>154</v>
-      </c>
-      <c r="G11" t="s">
-        <v>155</v>
-      </c>
-      <c r="H11" t="s">
-        <v>156</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>
@@ -2995,10 +3031,10 @@
         <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q11" t="s">
         <v>33</v>
@@ -3007,81 +3043,84 @@
         <v>34</v>
       </c>
       <c r="S11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V11">
         <v>2</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y11" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA11" t="s">
         <v>161</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AB11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>162</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="B12" t="s">
         <v>163</v>
       </c>
-      <c r="AB11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" t="s">
-        <v>165</v>
-      </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1">
         <v>42517</v>
       </c>
       <c r="F12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I12" t="s">
         <v>25</v>
@@ -3102,10 +3141,10 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q12" t="s">
         <v>33</v>
@@ -3114,69 +3153,72 @@
         <v>34</v>
       </c>
       <c r="S12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="T12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V12">
         <v>4</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X12" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z12" t="s">
         <v>172</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AA12" t="s">
         <v>173</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AB12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>174</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="B13" t="s">
         <v>175</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" t="s">
-        <v>177</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -3185,13 +3227,13 @@
         <v>42518</v>
       </c>
       <c r="F13" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" t="s">
         <v>178</v>
-      </c>
-      <c r="G13" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" t="s">
-        <v>180</v>
       </c>
       <c r="I13" t="s">
         <v>25</v>
@@ -3212,10 +3254,10 @@
         <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="P13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q13" t="s">
         <v>33</v>
@@ -3224,69 +3266,69 @@
         <v>34</v>
       </c>
       <c r="S13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="T13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="V13">
         <v>3</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X13" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z13" t="s">
         <v>185</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA13" t="s">
         <v>186</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AB13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF13" t="s">
         <v>187</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AH13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>188</v>
       </c>
-      <c r="AB13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF13" t="s">
+      <c r="B14" t="s">
         <v>189</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" t="s">
-        <v>191</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -3295,13 +3337,13 @@
         <v>42517</v>
       </c>
       <c r="F14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" t="s">
         <v>192</v>
-      </c>
-      <c r="G14" t="s">
-        <v>193</v>
-      </c>
-      <c r="H14" t="s">
-        <v>194</v>
       </c>
       <c r="I14" t="s">
         <v>25</v>
@@ -3322,10 +3364,10 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q14" t="s">
         <v>33</v>
@@ -3334,69 +3376,69 @@
         <v>34</v>
       </c>
       <c r="S14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="T14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V14">
         <v>4</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X14" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z14" t="s">
         <v>199</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>200</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AB14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>201</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="B15" t="s">
         <v>202</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>189</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15" t="s">
-        <v>204</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -3405,13 +3447,13 @@
         <v>42518</v>
       </c>
       <c r="F15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
         <v>205</v>
-      </c>
-      <c r="G15" t="s">
-        <v>206</v>
-      </c>
-      <c r="H15" t="s">
-        <v>207</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
@@ -3432,10 +3474,10 @@
         <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="P15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q15" t="s">
         <v>33</v>
@@ -3444,69 +3486,72 @@
         <v>34</v>
       </c>
       <c r="S15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="T15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="V15">
         <v>4</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y15" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA15" t="s">
         <v>211</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AB15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>212</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="B16" t="s">
         <v>213</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>214</v>
-      </c>
-      <c r="B16" t="s">
-        <v>215</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -3515,13 +3560,13 @@
         <v>42518</v>
       </c>
       <c r="F16" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" t="s">
         <v>216</v>
-      </c>
-      <c r="G16" t="s">
-        <v>217</v>
-      </c>
-      <c r="H16" t="s">
-        <v>218</v>
       </c>
       <c r="I16" t="s">
         <v>25</v>
@@ -3542,10 +3587,10 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Q16" t="s">
         <v>33</v>
@@ -3554,69 +3599,72 @@
         <v>34</v>
       </c>
       <c r="S16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="T16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="V16">
         <v>2</v>
       </c>
       <c r="W16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X16" t="s">
         <v>57</v>
       </c>
-      <c r="X16" t="s">
-        <v>58</v>
-      </c>
       <c r="Y16" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA16" t="s">
         <v>223</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AB16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>224</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="B17" t="s">
         <v>225</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>226</v>
-      </c>
-      <c r="B17" t="s">
-        <v>227</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -3625,13 +3673,13 @@
         <v>42636</v>
       </c>
       <c r="F17" t="s">
+        <v>226</v>
+      </c>
+      <c r="G17" t="s">
+        <v>227</v>
+      </c>
+      <c r="H17" t="s">
         <v>228</v>
-      </c>
-      <c r="G17" t="s">
-        <v>229</v>
-      </c>
-      <c r="H17" t="s">
-        <v>230</v>
       </c>
       <c r="I17" t="s">
         <v>25</v>
@@ -3652,10 +3700,10 @@
         <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Q17" t="s">
         <v>33</v>
@@ -3664,69 +3712,72 @@
         <v>34</v>
       </c>
       <c r="S17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V17">
         <v>3</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X17" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z17" t="s">
         <v>233</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AA17" t="s">
         <v>234</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AB17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>235</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="B18" t="s">
         <v>236</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B18" t="s">
-        <v>238</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -3735,13 +3786,13 @@
         <v>42472</v>
       </c>
       <c r="F18" t="s">
+        <v>237</v>
+      </c>
+      <c r="G18" t="s">
+        <v>238</v>
+      </c>
+      <c r="H18" t="s">
         <v>239</v>
-      </c>
-      <c r="G18" t="s">
-        <v>240</v>
-      </c>
-      <c r="H18" t="s">
-        <v>241</v>
       </c>
       <c r="I18" t="s">
         <v>25</v>
@@ -3762,10 +3813,10 @@
         <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q18" t="s">
         <v>33</v>
@@ -3774,69 +3825,72 @@
         <v>34</v>
       </c>
       <c r="S18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="T18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="V18">
         <v>4</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y18" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA18" t="s">
         <v>246</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AB18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE18" t="s">
         <v>247</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AF18" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>248</v>
       </c>
-      <c r="AB18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE18" t="s">
+      <c r="B19" t="s">
         <v>249</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>250</v>
-      </c>
-      <c r="B19" t="s">
-        <v>251</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -3845,13 +3899,13 @@
         <v>42517</v>
       </c>
       <c r="F19" t="s">
+        <v>250</v>
+      </c>
+      <c r="G19" t="s">
+        <v>251</v>
+      </c>
+      <c r="H19" t="s">
         <v>252</v>
-      </c>
-      <c r="G19" t="s">
-        <v>253</v>
-      </c>
-      <c r="H19" t="s">
-        <v>254</v>
       </c>
       <c r="I19" t="s">
         <v>25</v>
@@ -3872,10 +3926,10 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Q19" t="s">
         <v>33</v>
@@ -3884,81 +3938,84 @@
         <v>34</v>
       </c>
       <c r="S19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="T19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="V19">
         <v>4</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X19" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z19" t="s">
         <v>258</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="AA19" t="s">
         <v>259</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AB19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>260</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="B20" t="s">
         <v>261</v>
       </c>
-      <c r="AB19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>249</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>262</v>
-      </c>
-      <c r="B20" t="s">
-        <v>263</v>
-      </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1">
         <v>42518</v>
       </c>
       <c r="F20" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" t="s">
+        <v>263</v>
+      </c>
+      <c r="H20" t="s">
         <v>264</v>
-      </c>
-      <c r="G20" t="s">
-        <v>265</v>
-      </c>
-      <c r="H20" t="s">
-        <v>266</v>
       </c>
       <c r="I20" t="s">
         <v>25</v>
@@ -3979,10 +4036,10 @@
         <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q20" t="s">
         <v>33</v>
@@ -3991,63 +4048,66 @@
         <v>34</v>
       </c>
       <c r="S20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="V20">
         <v>2</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y20" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE20" t="s">
         <v>271</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AF20" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>272</v>
       </c>
-      <c r="AB20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE20" t="s">
+      <c r="B21" t="s">
         <v>273</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>274</v>
-      </c>
-      <c r="B21" t="s">
-        <v>275</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -4056,13 +4116,13 @@
         <v>42833</v>
       </c>
       <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>275</v>
+      </c>
+      <c r="H21" t="s">
         <v>276</v>
-      </c>
-      <c r="G21" t="s">
-        <v>277</v>
-      </c>
-      <c r="H21" t="s">
-        <v>278</v>
       </c>
       <c r="I21" t="s">
         <v>25</v>
@@ -4083,10 +4143,10 @@
         <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q21" t="s">
         <v>33</v>
@@ -4095,78 +4155,81 @@
         <v>34</v>
       </c>
       <c r="S21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="T21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="V21">
         <v>4</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X21" t="s">
+        <v>281</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z21" t="s">
         <v>283</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="AB21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>271</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>284</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="B22" t="s">
         <v>285</v>
       </c>
-      <c r="AB21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>273</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
         <v>286</v>
-      </c>
-      <c r="B22" t="s">
-        <v>287</v>
-      </c>
-      <c r="C22" t="s">
-        <v>288</v>
       </c>
       <c r="D22" s="1">
         <v>42636</v>
       </c>
       <c r="F22" t="s">
+        <v>287</v>
+      </c>
+      <c r="G22" t="s">
+        <v>288</v>
+      </c>
+      <c r="H22" t="s">
         <v>289</v>
-      </c>
-      <c r="G22" t="s">
-        <v>290</v>
-      </c>
-      <c r="H22" t="s">
-        <v>291</v>
       </c>
       <c r="I22" t="s">
         <v>25</v>
@@ -4187,10 +4250,10 @@
         <v>30</v>
       </c>
       <c r="O22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="P22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q22" t="s">
         <v>33</v>
@@ -4199,63 +4262,66 @@
         <v>34</v>
       </c>
       <c r="S22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="T22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="V22">
         <v>1</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X22" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z22" t="s">
         <v>296</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="AB22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>297</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="B23" t="s">
         <v>298</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>299</v>
-      </c>
-      <c r="B23" t="s">
-        <v>300</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -4264,13 +4330,13 @@
         <v>42833</v>
       </c>
       <c r="F23" t="s">
+        <v>299</v>
+      </c>
+      <c r="G23" t="s">
+        <v>300</v>
+      </c>
+      <c r="H23" t="s">
         <v>301</v>
-      </c>
-      <c r="G23" t="s">
-        <v>302</v>
-      </c>
-      <c r="H23" t="s">
-        <v>303</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -4291,10 +4357,10 @@
         <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Q23" t="s">
         <v>33</v>
@@ -4303,66 +4369,69 @@
         <v>34</v>
       </c>
       <c r="S23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="T23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V23">
         <v>3</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X23" t="s">
+        <v>306</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>308</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="B24" t="s">
         <v>309</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>311</v>
-      </c>
-      <c r="B24" t="s">
-        <v>312</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -4371,13 +4440,13 @@
         <v>43192</v>
       </c>
       <c r="F24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H24" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I24" t="s">
         <v>25</v>
@@ -4398,10 +4467,10 @@
         <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="P24" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="Q24" t="s">
         <v>33</v>
@@ -4410,66 +4479,69 @@
         <v>34</v>
       </c>
       <c r="S24" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="T24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="V24">
         <v>2</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y24" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>317</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>319</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="B25" t="s">
         <v>320</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>321</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>310</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK24" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>322</v>
-      </c>
-      <c r="B25" t="s">
-        <v>323</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -4478,13 +4550,13 @@
         <v>42857</v>
       </c>
       <c r="F25" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G25" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H25" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
@@ -4505,10 +4577,10 @@
         <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P25" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="Q25" t="s">
         <v>33</v>
@@ -4517,58 +4589,61 @@
         <v>34</v>
       </c>
       <c r="S25" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="T25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="V25">
         <v>4</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y25" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Z25" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AA25" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG25" t="s">
         <v>332</v>
       </c>
-      <c r="AB25" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>310</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>81</v>
-      </c>
       <c r="AH25" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="AI25" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AJ25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AK25" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="AL25" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top level menu, Restriction based data filtration, reports, new home page view and, issue fixes.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="335">
   <si>
     <t>Title</t>
   </si>
@@ -1021,6 +1021,9 @@
   </si>
   <si>
     <t>Marantz 661</t>
+  </si>
+  <si>
+    <t>Little Thunder, Julie Pearson;Finchum, Tanya; Bishop, Alex</t>
   </si>
 </sst>
 </file>
@@ -1834,12 +1837,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF29" sqref="AF29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1981,7 +1986,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>334</v>
       </c>
       <c r="D2" s="1">
         <v>42518</v>

</xml_diff>

<commit_message>
Process improvements, bug fixes in records import using excel file.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="433">
   <si>
     <t>Title</t>
   </si>
@@ -162,27 +162,18 @@
     <t>Restriction Notes</t>
   </si>
   <si>
-    <t>Recording Format</t>
-  </si>
-  <si>
     <t>Interviewer Notes</t>
   </si>
   <si>
     <t>Sent Out</t>
   </si>
   <si>
-    <t>Transcription Status</t>
-  </si>
-  <si>
     <t>Access Media Status</t>
   </si>
   <si>
     <t>Born digital</t>
   </si>
   <si>
-    <t>On CONTENTdm</t>
-  </si>
-  <si>
     <t>Madison</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>audio and video</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -762,9 +750,6 @@
     <t>St. John's, Antigua, immigrants, Tulsa, racism, nursing, black nurses, Okemah lynching, Laura Nelson, LD Nelson, Jane Crow</t>
   </si>
   <si>
-    <t xml:space="preserve">audio   </t>
-  </si>
-  <si>
     <t>Oral history interview with Charles Burris</t>
   </si>
   <si>
@@ -834,9 +819,6 @@
     <t>Women in the workforce, education, aspiration</t>
   </si>
   <si>
-    <t>audio</t>
-  </si>
-  <si>
     <t>Oral history interview with Robert Buzzard</t>
   </si>
   <si>
@@ -1024,6 +1006,318 @@
   </si>
   <si>
     <t>Little Thunder, Julie Pearson;Finchum, Tanya; Bishop, Alex</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Oral history interview with Nina Provence</t>
+  </si>
+  <si>
+    <t>Provence, Nina</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; World War (1939-1945)</t>
+  </si>
+  <si>
+    <t>WWII; Free time; Musical performance</t>
+  </si>
+  <si>
+    <t>Nina Provence recalled her childhood and arranged marriage. She discussed being the only woman working in her town's post office during World War II, her role in the aftermath of the President John F. Kennedy assassination, and living in California during an earthquake. Nina recalled seeing her first airplane and first car as well as a few home remedies. She spoke about playing the piano, her daily routine, and her life at 100 years of age.</t>
+  </si>
+  <si>
+    <t>The Oklahoma 100 Year Life Collection is a joint effort between the Oklahoma Oral History Research Program and the Oklahoma State University College of Human Sciences featuring interviews with citizens of Oklahoma who have lived 100 years or more. In addition to the rich history, this project provides a venue for increasing awareness of the value of a long-lived life by recording, preserving, and making information about Oklahoma's centenarians accessible to scholars, researchers, and other interested persons.</t>
+  </si>
+  <si>
+    <t>transcripts; sound recordings; digital images</t>
+  </si>
+  <si>
+    <t>text; sound; image</t>
+  </si>
+  <si>
+    <t>Oklahoma 100 Year Life</t>
+  </si>
+  <si>
+    <t>Oklahoma; Stillwater, Oklahoma</t>
+  </si>
+  <si>
+    <t>1920-2013</t>
+  </si>
+  <si>
+    <t>OHY_001</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>TF AC, TF E1, JN E2, draft mailed 6/13, complete 11/13</t>
+  </si>
+  <si>
+    <t>Canon XA20</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Oral history interview with Russell Pierson</t>
+  </si>
+  <si>
+    <t>Pierson, Russell</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Agricultural services</t>
+  </si>
+  <si>
+    <t>College track; Radio news; Country living</t>
+  </si>
+  <si>
+    <t>Russell Pierson, an Oklahoma agricultural icon, shared memories of his childhood on the family farm and the path he took to get an education at Oklahoma A&amp;M College (now Oklahoma State University). He spoke about his career in agriculture from being a county agricultural agent to owning a seed business to farm broadcasting. Russell also discussed his family history, daily routine, and successful long marriage.</t>
+  </si>
+  <si>
+    <t>transcripts; video recordings; digital images</t>
+  </si>
+  <si>
+    <t>Mangum, Oklahoma; Garvin County, Oklahoma</t>
+  </si>
+  <si>
+    <t>1916-2013</t>
+  </si>
+  <si>
+    <t>OHY_002</t>
+  </si>
+  <si>
+    <t>JoBeth</t>
+  </si>
+  <si>
+    <t>TF AC, TF E1, JN E2, draft mailed 7/13, complete 11/13</t>
+  </si>
+  <si>
+    <t>Oral history interview with Vance Trimble</t>
+  </si>
+  <si>
+    <t>Trimble, Vance H.</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Journalists; Newspaper publishing</t>
+  </si>
+  <si>
+    <t>News media; Writers; 1930s</t>
+  </si>
+  <si>
+    <t>Vance Trimble, a Pulitzer Prize winning journalist, discussed his lifelong career in journalism and his mentors, Paul Miller and Walker Stone. He also spoke about the subject of several books including Happy Chandler, Sam Walton, E.W. Scripts, and Chris Whittle.  He further discussed his memorial to his wife in Wewoka, Oklahoma. Vance also shared his daily routine and explained what life is like at 100 years of age.</t>
+  </si>
+  <si>
+    <t>Wewoka, Oklahoma; Houston, Texas; Washington, DC; Covington, Kentucky</t>
+  </si>
+  <si>
+    <t>1919-2013</t>
+  </si>
+  <si>
+    <t>OHY_003</t>
+  </si>
+  <si>
+    <t>Jo Beth</t>
+  </si>
+  <si>
+    <t>TF AC, TF E1, JN E2, draft mailed 8/13, complete 11/13</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Oral history interview with Stella Carroll</t>
+  </si>
+  <si>
+    <t>Carroll, Stella</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Dairy farming; Longevity</t>
+  </si>
+  <si>
+    <t>Childhood; Work; Daily activities</t>
+  </si>
+  <si>
+    <t>Stella Hanson Carroll shared memories of her childhood from living on a farm to moving to town. She discussed growing up around the University of Central Oklahoma, marrying, and operating a dairy farm. Stella also spoke about life at 102 and her daily activities, especially her love of reading.</t>
+  </si>
+  <si>
+    <t>Edmond, Oklahoma; Oklahoma County, Oklahoma</t>
+  </si>
+  <si>
+    <t>1919-2015</t>
+  </si>
+  <si>
+    <t>OHY_108</t>
+  </si>
+  <si>
+    <t>TF AC, E1, draft mailed 5/16, complete 7/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edmond, OK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs. Carroll recalled fond memories of her father and of growing up in Edmond, Oklahoma. She spoke about being in the dairy business with her first husband and about life after his death. </t>
+  </si>
+  <si>
+    <t>Edmond (OK), rural life, farming, retirement</t>
+  </si>
+  <si>
+    <t>life at 100, early day Edmond (OK), depression</t>
+  </si>
+  <si>
+    <t>Oral history interview with Hershel Pence</t>
+  </si>
+  <si>
+    <t>Pence, Hershel</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Occupations; House painting</t>
+  </si>
+  <si>
+    <t>Childhood; WPA; Country living</t>
+  </si>
+  <si>
+    <t>Hershel Pence discussed his early childhood, losing his father at a young age, and helping to support the family. He spoke about the opportunity the Works Progress Administration provided him and how he worked as a carpenter for a while before moving into the business of painting houses and businesses. He also shared about his life at 104 and a few things that may have contributed to his long life.</t>
+  </si>
+  <si>
+    <t>Hugo, Oklahoma</t>
+  </si>
+  <si>
+    <t>1917-2016</t>
+  </si>
+  <si>
+    <t>OHY_109</t>
+  </si>
+  <si>
+    <t>Jenna</t>
+  </si>
+  <si>
+    <t>Hugo, OK</t>
+  </si>
+  <si>
+    <t>Mr. Pence talked about moving to Hugo, Oklahoma in 1918, at the age of 7, about his father's death when he was 13, and about raising cattle on the open range. He also talked about working for the WPA and helping to build the football stadium in Hugo.</t>
+  </si>
+  <si>
+    <t>Hugo (OK), farming, painting</t>
+  </si>
+  <si>
+    <t>Rural life, WPA, life at 100</t>
+  </si>
+  <si>
+    <t>Oral history interview with Leona McGarry</t>
+  </si>
+  <si>
+    <t>McGarry, Leona</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Farm life; Hobbies</t>
+  </si>
+  <si>
+    <t>Country living; Child raising; Independent living</t>
+  </si>
+  <si>
+    <t>Leona McGarry discussed living near Boswell, Oklahoma, from a young child to a centenarian. She spoke about rural life and learning to drive and paint late in life. Leona talked about her creative inspirations and described a typical day at her age.</t>
+  </si>
+  <si>
+    <t>Choctaw County, Oklahoma; Boswell, Oklahoma</t>
+  </si>
+  <si>
+    <t>1921-2016</t>
+  </si>
+  <si>
+    <t>OHY_110</t>
+  </si>
+  <si>
+    <t>TF AC, TF, E1, draft mailed 5/16, complete 9/16</t>
+  </si>
+  <si>
+    <t>Soper, OK</t>
+  </si>
+  <si>
+    <t>Mrs. McGarry talked about living her entire life in the Soper area, attending a one-room school, and getting married. She also talked about learning to drive and learning to paint, both after the age of 65.</t>
+  </si>
+  <si>
+    <t>Soper (OK), family, daily living</t>
+  </si>
+  <si>
+    <t>Life at 100, creativity, rural life</t>
+  </si>
+  <si>
+    <t>Oral history interview with Ruth Martin</t>
+  </si>
+  <si>
+    <t>Martin, Ruth</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Teachers</t>
+  </si>
+  <si>
+    <t>Great Depression; Daily activities; Church</t>
+  </si>
+  <si>
+    <t>Ruth Martin recalled attending a one-room school and moving because of the Depression. She discussed earning college degrees as a non-traditional student and going on to teach school for over twenty years. Ruth also shared what life at 100 is like for her.</t>
+  </si>
+  <si>
+    <t>Stillwater, Oklahoma; Bethany, Oklahoma</t>
+  </si>
+  <si>
+    <t>OHY_111</t>
+  </si>
+  <si>
+    <t>TF AC, E1, draft mailed 5/16, complete 6/16</t>
+  </si>
+  <si>
+    <t>Stillwater, OK</t>
+  </si>
+  <si>
+    <t>Ruth Martin spoke briefly about attending Pleasant Valley School, her parents losing their home during the Depression, and returning to college at 42.</t>
+  </si>
+  <si>
+    <t>The Depression, Stillwater, teaching, birdwatching</t>
+  </si>
+  <si>
+    <t>Life at 100, family, education</t>
+  </si>
+  <si>
+    <t>Oral history interview with Wavel Ashbaugh</t>
+  </si>
+  <si>
+    <t>Ashbaugh, Wavel</t>
+  </si>
+  <si>
+    <t>Centenarians; Older people; Dance</t>
+  </si>
+  <si>
+    <t>Childhood; Family history; Married life; Work</t>
+  </si>
+  <si>
+    <t>Wavel Davis Ashbaugh shared childhood memories of her parents, of attending Catholic schools, and of early day Tulsa, Oklahoma. She recalled how she met her husband, Marvin Ash, and how his work as a pianist led them to move to California. Wavel talked about working well over the age of ninety and about taking up competitive ballroom dancing in her sixties.</t>
+  </si>
+  <si>
+    <t>Tulsa, Oklahoma; California</t>
+  </si>
+  <si>
+    <t>1916-2016</t>
+  </si>
+  <si>
+    <t>OHY_112</t>
+  </si>
+  <si>
+    <t>TF AC, TF, E1, draft mailed 5/16, complete 7/16</t>
+  </si>
+  <si>
+    <t>Broken Arrow, OK</t>
+  </si>
+  <si>
+    <t>Ms. Ashbaugh recalled memories of growing up in Tulsa, attending boarding school, and meeting her husband. She talked about their life in California following WWII where he was a jazz pianist, recorded music, and worked with Walt Disney for a while. She shared stories about her love for dancing, especially the waltz.</t>
+  </si>
+  <si>
+    <t>Tulsa (Okla.), Creek Indian, school, dance</t>
+  </si>
+  <si>
+    <t>Ballroom dancing, pianist, California, life at 100</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1346,6 +1640,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1507,13 +1807,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1835,31 +2146,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="25.140625" customWidth="1"/>
     <col min="25" max="25" width="32.7109375" customWidth="1"/>
     <col min="26" max="26" width="61.7109375" customWidth="1"/>
     <col min="27" max="27" width="34.7109375" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="31" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.85546875" customWidth="1"/>
+    <col min="31" max="31" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.85546875" customWidth="1"/>
+    <col min="33" max="33" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1951,13 +2274,13 @@
         <v>46</v>
       </c>
       <c r="AE1" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>48</v>
@@ -1969,16 +2292,10 @@
         <v>50</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>53</v>
+        <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1986,7 +2303,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D2" s="1">
         <v>42518</v>
@@ -2034,64 +2351,58 @@
         <v>35</v>
       </c>
       <c r="T2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V2">
         <v>3</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z2" t="s">
         <v>56</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>57</v>
       </c>
-      <c r="Y2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG2" t="s">
         <v>60</v>
       </c>
-      <c r="AB2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>332</v>
-      </c>
       <c r="AH2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AI2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AK2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2147,84 +2458,78 @@
         <v>35</v>
       </c>
       <c r="T3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V3">
         <v>3</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" t="s">
         <v>56</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>57</v>
       </c>
-      <c r="Y3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG3" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AH3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="C4" t="s">
         <v>63</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
       </c>
       <c r="D4" s="1">
         <v>42517</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -2245,10 +2550,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q4" t="s">
         <v>33</v>
@@ -2257,72 +2562,66 @@
         <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="T4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="V4">
         <v>3</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG4" t="s">
         <v>75</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AH4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="B5" t="s">
         <v>77</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -2331,13 +2630,13 @@
         <v>42518</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -2358,7 +2657,7 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P5" t="s">
         <v>32</v>
@@ -2370,203 +2669,191 @@
         <v>34</v>
       </c>
       <c r="S5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="T5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V5">
         <v>2</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Y5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5">
+        <v>42678</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="G6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AB5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE5" t="s">
+      <c r="H6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V6" s="4">
+        <v>4</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
         <v>63</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1">
-        <v>42678</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" t="s">
-        <v>95</v>
-      </c>
-      <c r="P6" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" t="s">
-        <v>97</v>
-      </c>
-      <c r="T6" t="s">
-        <v>54</v>
-      </c>
-      <c r="U6" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6">
-        <v>4</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="X6" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
       </c>
       <c r="D7" s="1">
         <v>42518</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
@@ -2587,10 +2874,10 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="P7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q7" t="s">
         <v>33</v>
@@ -2599,84 +2886,78 @@
         <v>34</v>
       </c>
       <c r="S7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="V7">
         <v>4</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Y7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AA7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AB7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AC7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AE7" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
         <v>63</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>42517</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
@@ -2697,10 +2978,10 @@
         <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="P8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Q8" t="s">
         <v>33</v>
@@ -2709,72 +2990,66 @@
         <v>34</v>
       </c>
       <c r="S8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="T8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V8">
         <v>3</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
         <v>122</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" t="s">
-        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -2783,13 +3058,13 @@
         <v>42719</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I9" t="s">
         <v>25</v>
@@ -2810,10 +3085,10 @@
         <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="P9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q9" t="s">
         <v>33</v>
@@ -2822,72 +3097,66 @@
         <v>34</v>
       </c>
       <c r="S9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="T9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="U9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V9">
         <v>4</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X9" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>134</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="B10" t="s">
         <v>135</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" t="s">
-        <v>139</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -2896,13 +3165,13 @@
         <v>42517</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
@@ -2923,10 +3192,10 @@
         <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="P10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q10" t="s">
         <v>33</v>
@@ -2935,72 +3204,66 @@
         <v>34</v>
       </c>
       <c r="S10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="T10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V10">
         <v>4</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Y10" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
         <v>147</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" t="s">
-        <v>151</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -3009,13 +3272,13 @@
         <v>42518</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>
@@ -3036,10 +3299,10 @@
         <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="P11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q11" t="s">
         <v>33</v>
@@ -3048,84 +3311,81 @@
         <v>34</v>
       </c>
       <c r="S11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="T11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="V11">
         <v>2</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Y11" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
         <v>159</v>
       </c>
-      <c r="Z11" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" t="s">
-        <v>163</v>
-      </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1">
         <v>42517</v>
       </c>
       <c r="F12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I12" t="s">
         <v>25</v>
@@ -3146,10 +3406,10 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="P12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="Q12" t="s">
         <v>33</v>
@@ -3158,182 +3418,170 @@
         <v>34</v>
       </c>
       <c r="S12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="T12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="V12">
         <v>4</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X12" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="B13" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5">
+        <v>42518</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="G13" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AB12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>61</v>
+      <c r="H13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="V13" s="4">
+        <v>3</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK13" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1">
-        <v>42518</v>
-      </c>
-      <c r="F13" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" t="s">
-        <v>177</v>
-      </c>
-      <c r="H13" t="s">
-        <v>178</v>
-      </c>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" t="s">
-        <v>179</v>
-      </c>
-      <c r="P13" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" t="s">
-        <v>34</v>
-      </c>
-      <c r="S13" t="s">
-        <v>181</v>
-      </c>
-      <c r="T13" t="s">
-        <v>54</v>
-      </c>
-      <c r="U13" t="s">
-        <v>182</v>
-      </c>
-      <c r="V13">
-        <v>3</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="X13" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y13" t="s">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>184</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="B14" t="s">
         <v>185</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>186</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>187</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" t="s">
-        <v>189</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -3342,13 +3590,13 @@
         <v>42517</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I14" t="s">
         <v>25</v>
@@ -3369,10 +3617,10 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="P14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="Q14" t="s">
         <v>33</v>
@@ -3381,69 +3629,63 @@
         <v>34</v>
       </c>
       <c r="S14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V14">
         <v>4</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X14" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>197</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="B15" t="s">
         <v>198</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>199</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>200</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>187</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>201</v>
-      </c>
-      <c r="B15" t="s">
-        <v>202</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -3452,13 +3694,13 @@
         <v>42518</v>
       </c>
       <c r="F15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
@@ -3479,10 +3721,10 @@
         <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="P15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q15" t="s">
         <v>33</v>
@@ -3491,72 +3733,66 @@
         <v>34</v>
       </c>
       <c r="S15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="T15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="V15">
         <v>4</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X15" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG15" t="s">
         <v>75</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AH15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" t="s">
         <v>209</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>210</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" t="s">
-        <v>213</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -3565,13 +3801,13 @@
         <v>42518</v>
       </c>
       <c r="F16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I16" t="s">
         <v>25</v>
@@ -3592,10 +3828,10 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Q16" t="s">
         <v>33</v>
@@ -3604,72 +3840,66 @@
         <v>34</v>
       </c>
       <c r="S16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="T16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="V16">
         <v>2</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Y16" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>219</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" t="s">
         <v>221</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>222</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B17" t="s">
-        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -3678,13 +3908,13 @@
         <v>42636</v>
       </c>
       <c r="F17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I17" t="s">
         <v>25</v>
@@ -3705,10 +3935,10 @@
         <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="P17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q17" t="s">
         <v>33</v>
@@ -3717,72 +3947,66 @@
         <v>34</v>
       </c>
       <c r="S17" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="T17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V17">
         <v>3</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X17" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>231</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="B18" t="s">
         <v>232</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>233</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>234</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" t="s">
-        <v>236</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -3791,13 +4015,13 @@
         <v>42472</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I18" t="s">
         <v>25</v>
@@ -3818,10 +4042,10 @@
         <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P18" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="Q18" t="s">
         <v>33</v>
@@ -3830,72 +4054,66 @@
         <v>34</v>
       </c>
       <c r="S18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="T18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U18" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="V18">
         <v>4</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Y18" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" t="s">
         <v>244</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>245</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>247</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>248</v>
-      </c>
-      <c r="B19" t="s">
-        <v>249</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -3904,13 +4122,13 @@
         <v>42517</v>
       </c>
       <c r="F19" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G19" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H19" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I19" t="s">
         <v>25</v>
@@ -3931,10 +4149,10 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="P19" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Q19" t="s">
         <v>33</v>
@@ -3943,84 +4161,78 @@
         <v>34</v>
       </c>
       <c r="S19" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="T19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="V19">
         <v>4</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X19" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" t="s">
         <v>256</v>
       </c>
-      <c r="Y19" t="s">
-        <v>257</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>258</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>259</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>247</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>260</v>
-      </c>
-      <c r="B20" t="s">
-        <v>261</v>
-      </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1">
         <v>42518</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G20" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H20" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I20" t="s">
         <v>25</v>
@@ -4041,10 +4253,10 @@
         <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="P20" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="Q20" t="s">
         <v>33</v>
@@ -4053,66 +4265,60 @@
         <v>34</v>
       </c>
       <c r="S20" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="T20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U20" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="V20">
         <v>2</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y20" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="Z20" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="AB20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AE20" t="s">
-        <v>271</v>
+        <v>327</v>
       </c>
       <c r="AF20" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AG20" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="AH20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AI20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AK20" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B21" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -4121,13 +4327,13 @@
         <v>42833</v>
       </c>
       <c r="F21" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G21" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="H21" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I21" t="s">
         <v>25</v>
@@ -4148,10 +4354,10 @@
         <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="P21" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="Q21" t="s">
         <v>33</v>
@@ -4160,81 +4366,75 @@
         <v>34</v>
       </c>
       <c r="S21" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="T21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U21" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="V21">
         <v>4</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X21" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Y21" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="Z21" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="AB21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AE21" t="s">
-        <v>271</v>
+        <v>327</v>
       </c>
       <c r="AF21" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AG21" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="AH21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AI21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AK21" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL21" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C22" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D22" s="1">
         <v>42636</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G22" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="H22" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="I22" t="s">
         <v>25</v>
@@ -4255,10 +4455,10 @@
         <v>30</v>
       </c>
       <c r="O22" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="P22" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="Q22" t="s">
         <v>33</v>
@@ -4267,66 +4467,60 @@
         <v>34</v>
       </c>
       <c r="S22" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="T22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U22" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="V22">
         <v>1</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X22" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="Y22" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="Z22" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="AB22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AE22" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="AF22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AG22" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="AH22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AI22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AK22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B23" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -4335,13 +4529,13 @@
         <v>42833</v>
       </c>
       <c r="F23" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G23" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H23" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -4362,10 +4556,10 @@
         <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="P23" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="Q23" t="s">
         <v>33</v>
@@ -4374,69 +4568,63 @@
         <v>34</v>
       </c>
       <c r="S23" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="T23" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U23" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="V23">
         <v>3</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X23" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="Y23" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="Z23" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="AB23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AC23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AE23" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="AF23" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AG23" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="AH23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AI23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AK23" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL23" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -4445,13 +4633,13 @@
         <v>43192</v>
       </c>
       <c r="F24" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G24" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="H24" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="I24" t="s">
         <v>25</v>
@@ -4472,10 +4660,10 @@
         <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="P24" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="Q24" t="s">
         <v>33</v>
@@ -4484,69 +4672,63 @@
         <v>34</v>
       </c>
       <c r="S24" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="T24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="V24">
         <v>2</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X24" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="Y24" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="Z24" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="AA24" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="AB24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AC24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AE24" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="AF24" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AG24" t="s">
-        <v>332</v>
+        <v>75</v>
       </c>
       <c r="AH24" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="AI24" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="AJ24" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="AK24" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -4555,13 +4737,13 @@
         <v>42857</v>
       </c>
       <c r="F25" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G25" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
@@ -4582,10 +4764,10 @@
         <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="P25" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="Q25" t="s">
         <v>33</v>
@@ -4594,64 +4776,794 @@
         <v>34</v>
       </c>
       <c r="S25" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="T25" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="V25">
         <v>4</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Y25" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE25" t="s">
         <v>327</v>
       </c>
-      <c r="Z25" t="s">
-        <v>328</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>329</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>63</v>
-      </c>
       <c r="AF25" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>330</v>
+      </c>
+      <c r="B26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C26" t="s">
+        <v>280</v>
+      </c>
+      <c r="D26" s="7">
+        <v>41436</v>
+      </c>
+      <c r="F26" t="s">
+        <v>332</v>
+      </c>
+      <c r="G26" t="s">
         <v>333</v>
       </c>
-      <c r="AG25" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI25" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK25" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL25" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM25" t="s">
-        <v>62</v>
+      <c r="H26" t="s">
+        <v>334</v>
+      </c>
+      <c r="I26" t="s">
+        <v>335</v>
+      </c>
+      <c r="J26" t="s">
+        <v>336</v>
+      </c>
+      <c r="K26" t="s">
+        <v>337</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" t="s">
+        <v>338</v>
+      </c>
+      <c r="O26" t="s">
+        <v>339</v>
+      </c>
+      <c r="P26" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>33</v>
+      </c>
+      <c r="R26" t="s">
+        <v>34</v>
+      </c>
+      <c r="S26" t="s">
+        <v>341</v>
+      </c>
+      <c r="T26" t="s">
+        <v>342</v>
+      </c>
+      <c r="U26" t="s">
+        <v>343</v>
+      </c>
+      <c r="W26" s="2"/>
+      <c r="AB26" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>346</v>
+      </c>
+      <c r="B27" t="s">
+        <v>347</v>
+      </c>
+      <c r="C27" t="s">
+        <v>280</v>
+      </c>
+      <c r="D27" s="1">
+        <v>42858</v>
+      </c>
+      <c r="F27" t="s">
+        <v>348</v>
+      </c>
+      <c r="G27" t="s">
+        <v>349</v>
+      </c>
+      <c r="H27" t="s">
+        <v>350</v>
+      </c>
+      <c r="I27" t="s">
+        <v>335</v>
+      </c>
+      <c r="J27" t="s">
+        <v>351</v>
+      </c>
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" t="s">
+        <v>338</v>
+      </c>
+      <c r="O27" t="s">
+        <v>352</v>
+      </c>
+      <c r="P27" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>33</v>
+      </c>
+      <c r="R27" t="s">
+        <v>34</v>
+      </c>
+      <c r="S27" t="s">
+        <v>354</v>
+      </c>
+      <c r="T27" t="s">
+        <v>355</v>
+      </c>
+      <c r="U27" t="s">
+        <v>356</v>
+      </c>
+      <c r="W27" s="2"/>
+      <c r="AB27" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B28" t="s">
+        <v>358</v>
+      </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42859</v>
+      </c>
+      <c r="F28" t="s">
+        <v>359</v>
+      </c>
+      <c r="G28" t="s">
+        <v>360</v>
+      </c>
+      <c r="H28" t="s">
+        <v>361</v>
+      </c>
+      <c r="I28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J28" t="s">
+        <v>351</v>
+      </c>
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M28" t="s">
+        <v>338</v>
+      </c>
+      <c r="O28" t="s">
+        <v>362</v>
+      </c>
+      <c r="P28" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>33</v>
+      </c>
+      <c r="R28" t="s">
+        <v>34</v>
+      </c>
+      <c r="S28" t="s">
+        <v>364</v>
+      </c>
+      <c r="T28" t="s">
+        <v>365</v>
+      </c>
+      <c r="U28" t="s">
+        <v>366</v>
+      </c>
+      <c r="W28" s="2"/>
+      <c r="AB28" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D29" s="1">
+        <v>42346</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="W29" s="8"/>
+      <c r="X29" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" t="s">
+        <v>383</v>
+      </c>
+      <c r="C30" t="s">
+        <v>280</v>
+      </c>
+      <c r="D30" s="1">
+        <v>42401</v>
+      </c>
+      <c r="F30" t="s">
+        <v>384</v>
+      </c>
+      <c r="G30" t="s">
+        <v>385</v>
+      </c>
+      <c r="H30" t="s">
+        <v>386</v>
+      </c>
+      <c r="I30" t="s">
+        <v>335</v>
+      </c>
+      <c r="J30" t="s">
+        <v>351</v>
+      </c>
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" t="s">
+        <v>338</v>
+      </c>
+      <c r="O30" t="s">
+        <v>387</v>
+      </c>
+      <c r="P30" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>33</v>
+      </c>
+      <c r="R30" t="s">
+        <v>34</v>
+      </c>
+      <c r="S30" t="s">
+        <v>389</v>
+      </c>
+      <c r="T30" t="s">
+        <v>390</v>
+      </c>
+      <c r="U30" t="s">
+        <v>377</v>
+      </c>
+      <c r="W30" s="2"/>
+      <c r="X30" t="s">
+        <v>391</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" s="5">
+        <v>42401</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="W31" s="6"/>
+      <c r="X31" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y31" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="AA31" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB31" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC31" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE31" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF31" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK31" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>408</v>
+      </c>
+      <c r="B32" t="s">
+        <v>409</v>
+      </c>
+      <c r="C32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D32" s="1">
+        <v>42417</v>
+      </c>
+      <c r="F32" t="s">
+        <v>410</v>
+      </c>
+      <c r="G32" t="s">
+        <v>411</v>
+      </c>
+      <c r="H32" t="s">
+        <v>412</v>
+      </c>
+      <c r="I32" t="s">
+        <v>335</v>
+      </c>
+      <c r="J32" t="s">
+        <v>351</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" t="s">
+        <v>338</v>
+      </c>
+      <c r="O32" t="s">
+        <v>413</v>
+      </c>
+      <c r="P32" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>33</v>
+      </c>
+      <c r="R32" t="s">
+        <v>34</v>
+      </c>
+      <c r="S32" t="s">
+        <v>414</v>
+      </c>
+      <c r="T32" t="s">
+        <v>51</v>
+      </c>
+      <c r="U32" t="s">
+        <v>415</v>
+      </c>
+      <c r="W32" s="2"/>
+      <c r="X32" t="s">
+        <v>416</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>417</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>418</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>420</v>
+      </c>
+      <c r="B33" t="s">
+        <v>421</v>
+      </c>
+      <c r="C33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="1">
+        <v>42420</v>
+      </c>
+      <c r="F33" t="s">
+        <v>422</v>
+      </c>
+      <c r="G33" t="s">
+        <v>423</v>
+      </c>
+      <c r="H33" t="s">
+        <v>424</v>
+      </c>
+      <c r="I33" t="s">
+        <v>335</v>
+      </c>
+      <c r="J33" t="s">
+        <v>351</v>
+      </c>
+      <c r="K33" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" t="s">
+        <v>338</v>
+      </c>
+      <c r="O33" t="s">
+        <v>425</v>
+      </c>
+      <c r="P33" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>33</v>
+      </c>
+      <c r="R33" t="s">
+        <v>34</v>
+      </c>
+      <c r="S33" t="s">
+        <v>427</v>
+      </c>
+      <c r="T33" t="s">
+        <v>390</v>
+      </c>
+      <c r="U33" t="s">
+        <v>428</v>
+      </c>
+      <c r="W33" s="2"/>
+      <c r="X33" t="s">
+        <v>429</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>430</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>431</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>432</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Advanced settings, delete records and bug fixes.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -1413,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,7 +1763,7 @@
         <v>45</v>
       </c>
       <c r="AK3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL3" t="s">
         <v>44</v>
@@ -1853,7 +1853,7 @@
         <v>45</v>
       </c>
       <c r="AK4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL4" t="s">
         <v>44</v>
@@ -1943,7 +1943,7 @@
         <v>45</v>
       </c>
       <c r="AK5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL5" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Modify collection ,subseries records with details, improve export and bug fixed.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/cms_sample.xlsx
+++ b/src/WpfApp/Assets/cms_sample.xlsx
@@ -1414,13 +1414,13 @@
   <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2:AK5"/>
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1449,6 +1449,7 @@
     <col min="32" max="32" width="22.85546875" customWidth="1"/>
     <col min="33" max="33" width="18.85546875" customWidth="1"/>
     <col min="35" max="35" width="20.85546875" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1670,7 +1671,7 @@
         <v>47</v>
       </c>
       <c r="AJ2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AK2" t="s">
         <v>45</v>

</xml_diff>